<commit_message>
Ignore notes that have same title and content on import
</commit_message>
<xml_diff>
--- a/app/translations.xlsx
+++ b/app/translations.xlsx
@@ -23601,28 +23601,28 @@
     <t>Duplicate</t>
   </si>
   <si>
-    <t>duplicated_notes_PLURALS_few</t>
-  </si>
-  <si>
-    <t>duplicated_notes_PLURALS_many</t>
-  </si>
-  <si>
-    <t>duplicated_notes_PLURALS_one</t>
-  </si>
-  <si>
-    <t>Duplicated %1$d note</t>
-  </si>
-  <si>
-    <t>duplicated_notes_PLURALS_other</t>
-  </si>
-  <si>
-    <t>Duplicated %1$d notes</t>
-  </si>
-  <si>
-    <t>duplicated_notes_PLURALS_two</t>
-  </si>
-  <si>
-    <t>duplicated_notes_PLURALS_zero</t>
+    <t>duplicates_PLURALS_few</t>
+  </si>
+  <si>
+    <t>duplicates_PLURALS_many</t>
+  </si>
+  <si>
+    <t>duplicates_PLURALS_one</t>
+  </si>
+  <si>
+    <t>%1$d duplicate</t>
+  </si>
+  <si>
+    <t>duplicates_PLURALS_other</t>
+  </si>
+  <si>
+    <t>%1$d duplicates</t>
+  </si>
+  <si>
+    <t>duplicates_PLURALS_two</t>
+  </si>
+  <si>
+    <t>duplicates_PLURALS_zero</t>
   </si>
   <si>
     <t>edit</t>

</xml_diff>